<commit_message>
csv tablename duplication fix
csv tablename duplication fix
</commit_message>
<xml_diff>
--- a/download/header4/data.xlsx
+++ b/download/header4/data.xlsx
@@ -1,53 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\20230228_pythonReport\_git\report_python\download\header4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678DEECA-96C5-4838-9A1C-F9F65233D60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="2325" windowWidth="22905" windowHeight="12360" tabRatio="459" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4860" yWindow="2325" windowWidth="22905" windowHeight="12360" tabRatio="459" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,24 +56,128 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mytable" displayName="mytable" ref="A8:F1244" headerRowCount="1">
+  <autoFilter ref="A8:F1244"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Device"/>
+    <tableColumn id="2" name="Asset"/>
+    <tableColumn id="3" name="Last Date"/>
+    <tableColumn id="4" name="Last Update"/>
+    <tableColumn id="5" name="Location"/>
+    <tableColumn id="6" name="Remarque"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="2023-05-12-07-55-17" displayName="2023-05-12-07-55-17" ref="A8:F8" headerRowCount="1">
+  <autoFilter ref="A8:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Device"/>
+    <tableColumn id="2" name="Asset"/>
+    <tableColumn id="3" name="Last Date"/>
+    <tableColumn id="4" name="Last Update"/>
+    <tableColumn id="5" name="Location"/>
+    <tableColumn id="6" name="Remarque"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="2023-05-12-07-55-30" displayName="2023-05-12-07-55-30" ref="A8:F8" headerRowCount="1">
+  <autoFilter ref="A8:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Device"/>
+    <tableColumn id="2" name="Asset"/>
+    <tableColumn id="3" name="Last Date"/>
+    <tableColumn id="4" name="Last Update"/>
+    <tableColumn id="5" name="Location"/>
+    <tableColumn id="6" name="Remarque"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,56 +464,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="53.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="53.5703125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="14.28515625" customWidth="1" min="6" max="7"/>
+    <col width="12.85546875" customWidth="1" min="8" max="8"/>
+    <col width="12.5703125" customWidth="1" min="9" max="9"/>
+    <col width="13.42578125" customWidth="1" min="11" max="11"/>
+    <col width="22.140625" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>KAMOTO COPPER COMPANY OFFLINE DEVICES</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2023-05-12 07:55:30</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Clients: KAMOTO COPPER COMPANY</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="16.5" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Max Hours: 96</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Schedule: VEHICLES OFFLINE REPORT</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>KAMOTO COPPER COMPANY</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Device</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Asset</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Last Date</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Last Update</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Remarque</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <tableParts count="3">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>